<commit_message>
definitivo mainpy -aquivo com add detlahes extars e pesquisa de variaveiws, falta ajeitar a responsividade apra se adequar a variaws telas
</commit_message>
<xml_diff>
--- a/pronto para apresentar/livros.xlsx
+++ b/pronto para apresentar/livros.xlsx
@@ -1,80 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Virgínia Sobral\Downloads\pronto para apresentar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Memorias postumas de Bras Cubas</t>
-  </si>
-  <si>
-    <t>Letras</t>
-  </si>
-  <si>
-    <t>Macahdo De Axís</t>
-  </si>
-  <si>
-    <t>Autor difunto escreve sua vida aprtir da morte ate seu nascimento</t>
-  </si>
-  <si>
-    <t>sim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loacalizado na seçaõ ab da slaa a4, coletado no dia dez de dezembor de dois mil e vinte, 10/12/2020.
-</t>
-  </si>
-  <si>
-    <t>1520</t>
-  </si>
-  <si>
-    <t>o menino de pijama amarelo</t>
-  </si>
-  <si>
-    <t>Seguinte</t>
-  </si>
-  <si>
-    <t>não</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loacalizado na seçaõ ab da slaa a4, coletado no dia dez de dezembor de dois mil e vintye dois, livro publicado em 11 de outubro de 2007., numero de págiunas 192. Dimensões 20,8 x 13, 8 x 1,2 cm.
-</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,68 +408,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" t="n">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Memorias postumas de Bras Cubas</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Letras</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Macahdo De Axís</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Autor difunto escreve sua vida aprtir da morte ate seu nascimento</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loacalizado na seçaõ ab da slaa a4, coletado no dia dez de dezembor de dois mil e vinte, 10/12/2020.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1520</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>o menino de pijama amarelo</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Seguinte</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Macahdo De Axís</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Autor difunto escreve sua vida aprtir da morte ate seu nascimento</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loacalizado na seçaõ ab da slaa a4, coletado no dia dez de dezembor de dois mil e vintye dois, livro publicado em 11 de outubro de 2007., numero de págiunas 192. Dimensões 20,8 x 13, 8 x 1,2 cm.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>manual de porgamaçaõ 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>letars</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Euclides</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>este e um 2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">extras
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>manual de porgamaçaõ 1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>letars</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Euclides</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>este e um 2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">extras
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>